<commit_message>
Insertion Excel to BDD
Finalisation proche : il faudra changer les noms de promo
</commit_message>
<xml_diff>
--- a/CONFIG/Liste_Salles.xlsx
+++ b/CONFIG/Liste_Salles.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GEII-S1-S2" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="142">
   <si>
     <t xml:space="preserve">Type</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t xml:space="preserve">CC3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM</t>
   </si>
   <si>
     <t xml:space="preserve">VE3</t>
@@ -735,7 +738,7 @@
   <dimension ref="A1:E120"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1948,10 +1951,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D124"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D75" activeCellId="0" sqref="D75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2029,1151 +2032,1165 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>65</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>64</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>65</v>
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="6" t="s">
+      <c r="A12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="1" t="s">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>67</v>
+      <c r="A16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="C21" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>70</v>
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="8" t="s">
         <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>71</v>
+      <c r="A30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>73</v>
+      <c r="A35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>74</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6" t="s">
+      <c r="A36" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>74</v>
+      <c r="A39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B40" s="6" t="s">
+      <c r="C40" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>76</v>
+      <c r="A43" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B44" s="6" t="s">
+      <c r="A44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44" s="8" t="s">
         <v>77</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>77</v>
+      <c r="A47" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="6" t="s">
+      <c r="D48" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>79</v>
+      <c r="A51" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="8" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="6" t="s">
+      <c r="C52" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="C56" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="6" t="s">
+      <c r="C57" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="8" t="s">
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>84</v>
+      <c r="A66" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" s="6" t="s">
+        <v>85</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="6" t="s">
+      <c r="C67" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="1" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>86</v>
+      <c r="C68" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D69" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5" t="s">
+      <c r="D70" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D70" s="1" t="s">
+      <c r="B71" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="C71" s="1" t="s">
-        <v>88</v>
+        <v>10</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>92</v>
+      <c r="A72" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>91</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C74" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B75" s="6" t="s">
+      <c r="D75" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>93</v>
+        <v>20</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>94</v>
+      <c r="A77" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="6" t="s">
+      <c r="A78" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>95</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B80" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B80" s="6" t="s">
-        <v>95</v>
-      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>95</v>
+      <c r="A81" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>97</v>
+      <c r="A82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>97</v>
+      <c r="A84" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B85" s="6" t="s">
+      <c r="A85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B85" s="8" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>98</v>
+      <c r="A87" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B88" s="6" t="s">
+      <c r="A88" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B88" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>99</v>
+      <c r="A91" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="6" t="s">
+      <c r="A92" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>100</v>
+      <c r="A93" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B94" s="6" t="s">
+      <c r="A94" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B94" s="8" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B98" s="8" t="s">
-        <v>101</v>
+      <c r="A98" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B99" s="6" t="s">
+      <c r="A99" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B103" s="8" t="s">
-        <v>102</v>
+      <c r="A103" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B104" s="6" t="s">
+      <c r="A104" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="8" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B108" s="8" t="s">
-        <v>103</v>
+      <c r="A108" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B109" s="6" t="s">
+      <c r="A109" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>104</v>
+      <c r="A112" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B112" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B113" s="6" t="s">
+      <c r="A113" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B113" s="8" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="14" t="s">
-        <v>4</v>
+      <c r="A114" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="14" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="5" t="s">
+      <c r="A116" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B116" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B116" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>105</v>
+      <c r="B117" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B118" s="6" t="s">
+      <c r="A118" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="14" t="s">
-        <v>11</v>
+      <c r="A119" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="5" t="s">
+      <c r="A121" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B121" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B122" s="8" t="s">
-        <v>106</v>
+      <c r="B122" s="6" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B123" s="8" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -3195,7 +3212,7 @@
   <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C7 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3224,7 +3241,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3232,7 +3249,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3240,7 +3257,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3248,7 +3265,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3256,7 +3273,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3264,7 +3281,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3272,10 +3289,10 @@
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3283,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3291,7 +3308,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3299,7 +3316,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3307,7 +3324,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
@@ -3318,7 +3335,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -3329,7 +3346,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>23</v>
@@ -3340,7 +3357,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>20</v>
@@ -3351,7 +3368,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>20</v>
@@ -3362,7 +3379,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>6</v>
@@ -3373,7 +3390,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
@@ -3384,7 +3401,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
@@ -3395,7 +3412,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3403,7 +3420,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3411,7 +3428,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -3422,7 +3439,7 @@
         <v>7</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>8</v>
@@ -3433,7 +3450,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>10</v>
@@ -3444,7 +3461,7 @@
         <v>11</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3452,7 +3469,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3460,7 +3477,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -3471,7 +3488,7 @@
         <v>7</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>8</v>
@@ -3482,7 +3499,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>10</v>
@@ -3493,7 +3510,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>20</v>
@@ -3504,7 +3521,7 @@
         <v>13</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>20</v>
@@ -3515,7 +3532,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -3526,7 +3543,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>8</v>
@@ -3537,7 +3554,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>10</v>
@@ -3548,10 +3565,10 @@
         <v>11</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3559,10 +3576,10 @@
         <v>13</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3570,7 +3587,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -3581,7 +3598,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>8</v>
@@ -3592,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>10</v>
@@ -3603,7 +3620,7 @@
         <v>11</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>12</v>
@@ -3614,7 +3631,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>12</v>
@@ -3625,7 +3642,7 @@
         <v>4</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>6</v>
@@ -3636,7 +3653,7 @@
         <v>7</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>8</v>
@@ -3647,7 +3664,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3655,7 +3672,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3663,7 +3680,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,7 +3688,7 @@
         <v>4</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>6</v>
@@ -3682,7 +3699,7 @@
         <v>7</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
@@ -3693,7 +3710,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>10</v>
@@ -3704,10 +3721,10 @@
         <v>11</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3715,10 +3732,10 @@
         <v>13</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3726,7 +3743,7 @@
         <v>4</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>6</v>
@@ -3737,7 +3754,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>8</v>
@@ -3748,7 +3765,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>10</v>
@@ -3759,10 +3776,10 @@
         <v>11</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3770,10 +3787,10 @@
         <v>13</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3781,7 +3798,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>10</v>
@@ -3792,7 +3809,7 @@
         <v>11</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>6</v>
@@ -3803,10 +3820,10 @@
         <v>13</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3814,10 +3831,10 @@
         <v>41</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3825,10 +3842,10 @@
         <v>13</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3836,7 +3853,7 @@
         <v>4</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3844,7 +3861,7 @@
         <v>7</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,7 +3869,7 @@
         <v>9</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3860,7 +3877,7 @@
         <v>11</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3868,7 +3885,7 @@
         <v>13</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3876,7 +3893,7 @@
         <v>7</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3884,7 +3901,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3892,7 +3909,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,7 +3917,7 @@
         <v>11</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3908,7 +3925,7 @@
         <v>13</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3916,7 +3933,7 @@
         <v>7</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3924,7 +3941,7 @@
         <v>4</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3932,7 +3949,7 @@
         <v>9</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3940,7 +3957,7 @@
         <v>11</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3948,7 +3965,7 @@
         <v>13</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3956,7 +3973,7 @@
         <v>9</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3964,7 +3981,7 @@
         <v>11</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3972,7 +3989,7 @@
         <v>13</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3980,7 +3997,7 @@
         <v>41</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3988,7 +4005,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4010,7 +4027,7 @@
   <dimension ref="A1:D92"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
+      <selection pane="topLeft" activeCell="A80" activeCellId="1" sqref="C7 A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4299,7 +4316,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -4310,7 +4327,7 @@
         <v>7</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>10</v>
@@ -4321,7 +4338,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>10</v>
@@ -4332,7 +4349,7 @@
         <v>11</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>12</v>
@@ -4343,13 +4360,13 @@
         <v>13</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4357,7 +4374,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
@@ -4368,7 +4385,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -4379,7 +4396,7 @@
         <v>11</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>12</v>
@@ -4390,7 +4407,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>12</v>
@@ -4536,7 +4553,7 @@
         <v>4</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4544,7 +4561,7 @@
         <v>7</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4552,7 +4569,7 @@
         <v>9</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4560,7 +4577,7 @@
         <v>13</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4623,7 +4640,7 @@
         <v>4</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4631,7 +4648,7 @@
         <v>7</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4647,7 +4664,7 @@
         <v>11</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4655,7 +4672,7 @@
         <v>13</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4663,7 +4680,7 @@
         <v>4</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>6</v>
@@ -4674,7 +4691,7 @@
         <v>7</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>10</v>
@@ -4685,7 +4702,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4693,7 +4710,7 @@
         <v>11</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>28</v>
@@ -4704,7 +4721,7 @@
         <v>13</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>30</v>
@@ -4783,7 +4800,7 @@
         <v>47</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4794,7 +4811,7 @@
         <v>47</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4906,8 +4923,8 @@
   </sheetPr>
   <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A79" activeCellId="0" sqref="A79"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A79" activeCellId="1" sqref="C7 A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4963,7 +4980,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>63</v>
@@ -4985,7 +5002,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>64</v>
@@ -5023,10 +5040,10 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5034,7 +5051,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5042,7 +5059,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5050,7 +5067,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -5061,7 +5078,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5069,7 +5086,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>23</v>
@@ -5080,7 +5097,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>20</v>
@@ -5091,7 +5108,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5099,7 +5116,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>10</v>
@@ -5110,7 +5127,7 @@
         <v>13</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -5121,7 +5138,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -5132,7 +5149,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>10</v>
@@ -5143,7 +5160,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>10</v>
@@ -5154,10 +5171,10 @@
         <v>11</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5165,10 +5182,10 @@
         <v>13</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5176,7 +5193,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -5187,7 +5204,7 @@
         <v>7</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>10</v>
@@ -5198,7 +5215,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>10</v>
@@ -5209,7 +5226,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>38</v>
@@ -5220,7 +5237,7 @@
         <v>13</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>38</v>
@@ -5231,7 +5248,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -5242,7 +5259,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>10</v>
@@ -5253,7 +5270,7 @@
         <v>9</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>10</v>
@@ -5264,10 +5281,10 @@
         <v>11</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5275,10 +5292,10 @@
         <v>13</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5286,7 +5303,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -5297,7 +5314,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>10</v>
@@ -5308,7 +5325,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>10</v>
@@ -5319,7 +5336,7 @@
         <v>11</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>12</v>
@@ -5330,7 +5347,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>12</v>
@@ -5341,7 +5358,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>6</v>
@@ -5352,7 +5369,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>10</v>
@@ -5363,7 +5380,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>10</v>
@@ -5374,10 +5391,10 @@
         <v>11</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5385,18 +5402,18 @@
         <v>13</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>6</v>
@@ -5407,7 +5424,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>8</v>
@@ -5418,7 +5435,7 @@
         <v>9</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>10</v>
@@ -5429,7 +5446,7 @@
         <v>13</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5437,7 +5454,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>6</v>
@@ -5448,7 +5465,7 @@
         <v>7</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>10</v>
@@ -5459,7 +5476,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>10</v>
@@ -5470,13 +5487,13 @@
         <v>11</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5484,13 +5501,13 @@
         <v>13</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5498,7 +5515,7 @@
         <v>4</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>6</v>
@@ -5509,7 +5526,7 @@
         <v>7</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>10</v>
@@ -5520,7 +5537,7 @@
         <v>9</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>10</v>
@@ -5531,10 +5548,10 @@
         <v>11</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5542,10 +5559,10 @@
         <v>13</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5553,7 +5570,7 @@
         <v>4</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>6</v>
@@ -5564,7 +5581,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>10</v>
@@ -5575,7 +5592,7 @@
         <v>9</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>10</v>
@@ -5586,10 +5603,10 @@
         <v>11</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5597,10 +5614,10 @@
         <v>13</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5608,7 +5625,7 @@
         <v>4</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>6</v>
@@ -5619,7 +5636,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>10</v>
@@ -5630,7 +5647,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>10</v>
@@ -5641,10 +5658,10 @@
         <v>11</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5652,10 +5669,10 @@
         <v>13</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5663,7 +5680,7 @@
         <v>4</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>6</v>
@@ -5674,7 +5691,7 @@
         <v>7</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>10</v>
@@ -5685,7 +5702,7 @@
         <v>9</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>10</v>
@@ -5696,10 +5713,10 @@
         <v>11</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5707,13 +5724,13 @@
         <v>13</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5721,13 +5738,13 @@
         <v>9</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5735,7 +5752,7 @@
         <v>11</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5743,10 +5760,10 @@
         <v>13</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5754,13 +5771,13 @@
         <v>9</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5768,13 +5785,13 @@
         <v>41</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5782,10 +5799,10 @@
         <v>13</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5793,7 +5810,7 @@
         <v>9</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5801,7 +5818,7 @@
         <v>11</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5809,7 +5826,7 @@
         <v>13</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5817,7 +5834,7 @@
         <v>41</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5825,7 +5842,7 @@
         <v>13</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5833,7 +5850,7 @@
         <v>4</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5841,7 +5858,7 @@
         <v>9</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5849,7 +5866,7 @@
         <v>11</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5857,7 +5874,7 @@
         <v>13</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5865,7 +5882,7 @@
         <v>9</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5873,15 +5890,15 @@
         <v>13</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5889,7 +5906,7 @@
         <v>7</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5897,7 +5914,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5905,7 +5922,7 @@
         <v>4</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5913,7 +5930,7 @@
         <v>7</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5921,7 +5938,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5929,7 +5946,7 @@
         <v>13</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5937,7 +5954,7 @@
         <v>4</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5945,7 +5962,7 @@
         <v>7</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5953,7 +5970,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5961,7 +5978,7 @@
         <v>13</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5969,7 +5986,7 @@
         <v>4</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5977,7 +5994,7 @@
         <v>7</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5985,7 +6002,7 @@
         <v>9</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5993,7 +6010,7 @@
         <v>11</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6001,7 +6018,7 @@
         <v>13</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6009,7 +6026,7 @@
         <v>4</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6017,7 +6034,7 @@
         <v>7</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6025,7 +6042,7 @@
         <v>9</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6033,7 +6050,7 @@
         <v>11</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6041,7 +6058,7 @@
         <v>13</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6049,7 +6066,7 @@
         <v>4</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6057,7 +6074,7 @@
         <v>7</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6065,7 +6082,7 @@
         <v>9</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6073,7 +6090,7 @@
         <v>11</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6081,7 +6098,7 @@
         <v>13</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6089,7 +6106,7 @@
         <v>4</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6097,7 +6114,7 @@
         <v>7</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6105,7 +6122,7 @@
         <v>9</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,7 +6130,7 @@
         <v>11</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6121,7 +6138,7 @@
         <v>13</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6129,7 +6146,7 @@
         <v>9</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6137,7 +6154,7 @@
         <v>4</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6145,7 +6162,7 @@
         <v>13</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6153,7 +6170,7 @@
         <v>41</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6161,7 +6178,7 @@
         <v>13</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>